<commit_message>
Initial commit of LLBv3 function tests
</commit_message>
<xml_diff>
--- a/Electronics/Low Level/Pin Mapping.xlsx
+++ b/Electronics/Low Level/Pin Mapping.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Projects/elcano/Electronics/Low Level v3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Projects/elcano/Electronics/Low Level/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28A8BB6-29E7-FF48-896E-DE48F8AC78D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DA4F3E-D6E7-1D40-96E8-D0AEABB52D7F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="440" windowWidth="25600" windowHeight="21160" xr2:uid="{2E9AF3F1-2BA1-F14D-8C1F-E5BC4609F5C6}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="19200" windowHeight="21160" xr2:uid="{2E9AF3F1-2BA1-F14D-8C1F-E5BC4609F5C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="215">
   <si>
     <t>PG5 ( OC0B )</t>
   </si>
@@ -672,6 +673,9 @@
   </si>
   <si>
     <t>E-stop (INT)</t>
+  </si>
+  <si>
+    <t>on board relay</t>
   </si>
 </sst>
 </file>
@@ -737,65 +741,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1166,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4080FD99-07AF-0640-A5AF-54DF0F777A9D}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1791,6 +1737,12 @@
       <c r="C51" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="D51" t="s">
+        <v>189</v>
+      </c>
+      <c r="E51" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
@@ -1802,12 +1754,6 @@
       <c r="C52" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D52" t="s">
-        <v>192</v>
-      </c>
-      <c r="E52" t="s">
-        <v>191</v>
-      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
@@ -1819,12 +1765,6 @@
       <c r="C53" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D53" t="s">
-        <v>189</v>
-      </c>
-      <c r="E53" t="s">
-        <v>210</v>
-      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
@@ -2042,6 +1982,12 @@
       </c>
       <c r="C71" s="2" t="s">
         <v>111</v>
+      </c>
+      <c r="D71" t="s">
+        <v>192</v>
+      </c>
+      <c r="E71" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -2462,7 +2408,7 @@
       <formula>NOT(ISERROR(SEARCH("PCINT",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18:C19 A24:C27 A20:XFD23 A1:XFD1 A2:D2 F2:XFD2 F24:XFD27 A3:XFD7 A9:XFD17 A8:D8 F8:XFD8 F18:XFD19 A28:XFD81 I82:XFD82 F82 A82:C86 D83:XFD83 D84:F86 I84:XFD86 A87:XFD1048576">
+  <conditionalFormatting sqref="A18:C19 A24:C27 A20:XFD23 A1:XFD1 A2:D2 F2:XFD2 F24:XFD27 A3:XFD7 A9:XFD17 A8:D8 F8:XFD8 F18:XFD19 I82:XFD82 F82 A82:C86 D83:XFD83 D84:F86 I84:XFD86 A87:XFD1048576 A54:XFD81 A53:D53 F53:XFD53 A28:XFD52">
     <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="PWM">
       <formula>NOT(ISERROR(SEARCH("PWM",A1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Corrected pin mapping document for steering PWM pin
</commit_message>
<xml_diff>
--- a/Electronics/Low Level/Pin Mapping.xlsx
+++ b/Electronics/Low Level/Pin Mapping.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Projects/elcano/Electronics/Low Level/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DA4F3E-D6E7-1D40-96E8-D0AEABB52D7F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1F9358-0267-D042-BF8D-D6F7818957B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="19200" windowHeight="21160" xr2:uid="{2E9AF3F1-2BA1-F14D-8C1F-E5BC4609F5C6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16780" windowHeight="20540" xr2:uid="{2E9AF3F1-2BA1-F14D-8C1F-E5BC4609F5C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1112,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4080FD99-07AF-0640-A5AF-54DF0F777A9D}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1322,6 +1321,12 @@
       <c r="C16" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="D16" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -1333,12 +1338,6 @@
       <c r="C17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D17" t="s">
-        <v>183</v>
-      </c>
-      <c r="E17" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
@@ -2403,12 +2402,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A18:C19 A89:C90 A24:C27 A91:D1048576 A1:D17 A88:D88 A20:D23 A28:D81 A82:C87 D83:D1048576">
+  <conditionalFormatting sqref="A89:C90 A24:C27 A91:D1048576 A88:D88 A20:D23 A28:D81 A82:C87 D83:D1048576 A17:C19 A1:D16">
     <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="PCINT">
       <formula>NOT(ISERROR(SEARCH("PCINT",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18:C19 A24:C27 A20:XFD23 A1:XFD1 A2:D2 F2:XFD2 F24:XFD27 A3:XFD7 A9:XFD17 A8:D8 F8:XFD8 F18:XFD19 I82:XFD82 F82 A82:C86 D83:XFD83 D84:F86 I84:XFD86 A87:XFD1048576 A54:XFD81 A53:D53 F53:XFD53 A28:XFD52">
+  <conditionalFormatting sqref="A24:C27 A20:XFD23 A1:XFD1 A2:D2 F2:XFD2 F24:XFD27 A3:XFD7 A8:D8 F8:XFD8 I82:XFD82 F82 A82:C86 D83:XFD83 D84:F86 I84:XFD86 A87:XFD1048576 A54:XFD81 A53:D53 F53:XFD53 A28:XFD52 A17:C19 F17:XFD19 A9:XFD16">
     <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="PWM">
       <formula>NOT(ISERROR(SEARCH("PWM",A1)))</formula>
     </cfRule>
@@ -2416,7 +2415,7 @@
       <formula>NOT(ISERROR(SEARCH("Digital Pin",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D17 D20:D23 D28:D81 D83:D1048576">
+  <conditionalFormatting sqref="D20:D23 D28:D81 D83:D1048576 D1:D16">
     <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="INT">
       <formula>NOT(ISERROR(SEARCH("INT",D1)))</formula>
     </cfRule>

</xml_diff>